<commit_message>
final edit of today, everything should work flawlessly on OS 2,9.X
</commit_message>
<xml_diff>
--- a/Fractions_AravaEtAll_Stims-Procs.xlsx
+++ b/Fractions_AravaEtAll_Stims-Procs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="695" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="748" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Size Pract" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,8 @@
     <sheet name="All_StimPairsX1.1" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="All_StimPairsX2" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="SizeTaskSound" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="FracTascSound" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="FracTaskSound" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="SizeTrainSound" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Area2Duration!$A$1:$L$109</definedName>
@@ -30,21 +31,24 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Frac Pract'!$AF$2:$AG$110</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Frac Pract'!$AF$2:$AG$110</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Frac Pract'!$AF$2:$AG$110</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Frac Pract'!$AF$2:$AG$110</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Frac Task'!$AF$2:$AG$110</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Frac Task'!$AF$2:$AG$110</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Frac Task'!$AF$2:$AG$110</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Frac Task'!$AF$2:$AG$110</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Frac Task'!$AF$2:$AG$110</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Frac Task'!$AF$2:$AG$110</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Area2Duration!$A$1:$L$109</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Area2Duration!$A$1:$L$109</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Area2Duration!$A$1:$L$109</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Area2Duration!$A$1:$L$109</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10659" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10859" uniqueCount="442">
   <si>
     <t>LeftStim</t>
   </si>
@@ -15934,7 +15938,7 @@
   </sheetPr>
   <dimension ref="A1:AI109"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N96" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -23905,8 +23909,8 @@
   </sheetPr>
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -30670,6 +30674,1273 @@
       </c>
       <c r="T109" s="0" t="n">
         <v>4508</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T20"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="0" t="n">
+        <v>3772</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>944</v>
+      </c>
+      <c r="Q1" s="0" t="n">
+        <v>2828</v>
+      </c>
+      <c r="R1" s="0" t="n">
+        <v>1060</v>
+      </c>
+      <c r="S1" s="0" t="n">
+        <v>662</v>
+      </c>
+      <c r="T1" s="0" t="n">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>1508</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>942</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>566</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>2652</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>664</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>2024</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>758</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>2060</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>1546</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1688</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>422</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>2472</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>1546</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>2652</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>664</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>1988</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>1508</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>942</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>1060</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>662</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>398</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>3772</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>944</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>2828</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>2920</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>1826</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>1094</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>1688</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>2434</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>1826</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>608</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>2024</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>4892</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>1224</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>3668</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>1060</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>662</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>1956</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>1222</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>734</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>2652</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>664</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>2024</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>758</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>2434</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>1826</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>1688</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>422</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>2920</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>1826</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>2652</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>664</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>1988</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>1956</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>1222</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>1060</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>662</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>398</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>4892</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>1224</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>3668</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>3368</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>2106</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>1262</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>1688</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>2808</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>2106</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>702</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>2024</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>6012</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>1504</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>4508</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>1060</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>662</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>2404</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>1502</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>902</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>2652</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <v>664</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>2024</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>758</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>2808</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <v>2106</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>1688</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>1266</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>422</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <v>3368</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>2106</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>1262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>